<commit_message>
Corte 2 - Entrega
</commit_message>
<xml_diff>
--- a/Proyecto ingeniera de software/Formulario_LOGT.xlsx
+++ b/Proyecto ingeniera de software/Formulario_LOGT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28619"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvggt-my.sharepoint.com/personal/cas23201_uvg_edu_gt/Documents/Semestre 5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvggt-my.sharepoint.com/personal/dele23202_uvg_edu_gt/Documents/Proyecto ingeniera de software/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="337" documentId="8_{4D551FD1-5DEF-4910-AB05-6E5111A06BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6A5EC35-B28B-4AC8-B9A2-D8C2E1E324ED}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="8_{4D551FD1-5DEF-4910-AB05-6E5111A06BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8D92A2F-0433-4B21-82AF-EE76EB6B2FAB}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" firstSheet="1" activeTab="3" xr2:uid="{5E260E09-10DD-455B-A3DA-77A9164E766C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{5E260E09-10DD-455B-A3DA-77A9164E766C}"/>
   </bookViews>
   <sheets>
     <sheet name="Roberto" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="120">
   <si>
     <t>Nombre</t>
   </si>
@@ -122,10 +122,58 @@
     <t>Creacion de los mapas de empatia de cada entrevistado</t>
   </si>
   <si>
+    <t>0 minutos</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Tienda</t>
+  </si>
+  <si>
+    <t>Implementó la interfaz de la tienda</t>
+  </si>
+  <si>
+    <t>2.5h</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>Desarrolló el formulario de contacto</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Configuró el panel de administración</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Implementó la gestión de productos en el dashboard</t>
+  </si>
+  <si>
     <t>Paula Daniela de León Godoy</t>
   </si>
   <si>
-    <t>1.2.2025</t>
+    <t>1 min</t>
+  </si>
+  <si>
+    <t>14 min</t>
+  </si>
+  <si>
+    <t>busqueda</t>
+  </si>
+  <si>
+    <t>se introduce los datos al documento sobre los usuarios</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>6-7 min</t>
   </si>
   <si>
     <t>entrevistas</t>
@@ -134,15 +182,69 @@
     <t>Se entrevistaron a usuarios extremos</t>
   </si>
   <si>
-    <t>3.2.2025</t>
+    <t>4.5 horas</t>
+  </si>
+  <si>
+    <t>8.2 horas</t>
+  </si>
+  <si>
+    <t>encripcion</t>
+  </si>
+  <si>
+    <t>Se creo el resumen completo de cada entrevista</t>
+  </si>
+  <si>
+    <t>2 horas</t>
+  </si>
+  <si>
+    <t>8 horas</t>
+  </si>
+  <si>
+    <t>mapas de empatia</t>
+  </si>
+  <si>
+    <t>Se crean los mapas de empatia para cada usuario</t>
+  </si>
+  <si>
+    <t>50 min</t>
+  </si>
+  <si>
+    <t>1.4 horas</t>
+  </si>
+  <si>
+    <t>0 min</t>
+  </si>
+  <si>
+    <t>Autenticación</t>
+  </si>
+  <si>
+    <t>Pensó en la lógica de autenticación de usuarios</t>
+  </si>
+  <si>
+    <t>Seguridad</t>
+  </si>
+  <si>
+    <t>Propuso medidas para la protección de datos</t>
+  </si>
+  <si>
+    <t>Usabilidad</t>
+  </si>
+  <si>
+    <t>Diseñó la estructura del formulario de inicio de sesión</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0 min</t>
+  </si>
+  <si>
+    <t>Reportes</t>
+  </si>
+  <si>
+    <t>Especificó los requerimientos para reportes de ventas</t>
   </si>
   <si>
     <t>Ricardo Arturo Godínez Sánchez</t>
   </si>
   <si>
-    <t>29/01/2025</t>
-  </si>
-  <si>
     <t>45 min</t>
   </si>
   <si>
@@ -155,18 +257,12 @@
     <t>Se realizo una entrevista a un usuario anónimo de la empresa que decidio permanecer anónima</t>
   </si>
   <si>
-    <t>0 min</t>
-  </si>
-  <si>
     <t>Se colocó en la selección de usuarios externos a la enmpresa correspondiente</t>
   </si>
   <si>
     <t>Creación de la codificación y resumen en el documento de canva para la empresa</t>
   </si>
   <si>
-    <t>5 min</t>
-  </si>
-  <si>
     <t>Creación del mapa de empatía de la empresa en el documento de miro</t>
   </si>
   <si>
@@ -188,45 +284,48 @@
     <t>Resumen del documento.</t>
   </si>
   <si>
+    <t>Backend</t>
+  </si>
+  <si>
+    <t>Implementó la lógica del estado del pedido</t>
+  </si>
+  <si>
+    <t>Configuró la seguridad en la base de datos</t>
+  </si>
+  <si>
+    <t>Optimización</t>
+  </si>
+  <si>
+    <t>Mejoró la eficiencia de las consultas</t>
+  </si>
+  <si>
+    <t>Pedidos</t>
+  </si>
+  <si>
+    <t>Validó la integración con los pedidos</t>
+  </si>
+  <si>
     <t>Vianka Vanessa Castro Ordoñez</t>
   </si>
   <si>
     <t>HORAS</t>
   </si>
   <si>
-    <t>25/1/2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Creación de documento </t>
   </si>
   <si>
-    <t>27/1/2025</t>
-  </si>
-  <si>
     <t>Modificación e implementación de formato además de colocar las preguntas de las entrevistas</t>
   </si>
   <si>
-    <t>28/1/2025</t>
-  </si>
-  <si>
     <t>Colocar nuevos usuarios internos, crear su AEIOU,sus entrevistas y sus QUE COMO y PORQUE</t>
   </si>
   <si>
-    <t>29/1/2025</t>
-  </si>
-  <si>
     <t>Comenzar el guión de entrevistas para internos y externos</t>
   </si>
   <si>
-    <t>30/1/2025</t>
-  </si>
-  <si>
     <t>Modificación de definición de usuarios internos</t>
   </si>
   <si>
-    <t>31/1/2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">Definir los perfiles que existen en la situación </t>
   </si>
   <si>
@@ -245,47 +344,68 @@
     <t>Ultimas modificaciones al documento y colocar imágenes de mapas de empatía.</t>
   </si>
   <si>
-    <t>encripcion</t>
-  </si>
-  <si>
-    <t>Se creo el resumen completo de cada entrevista</t>
-  </si>
-  <si>
-    <t>mapas de empatia</t>
-  </si>
-  <si>
-    <t>busqueda</t>
-  </si>
-  <si>
-    <t>se introduce los datos al documento sobre los usuarios</t>
-  </si>
-  <si>
-    <t>Se crean los mapas de empatia para cada usuario</t>
-  </si>
-  <si>
-    <t>6-7 min</t>
-  </si>
-  <si>
-    <t>1 min</t>
-  </si>
-  <si>
-    <t>14 min</t>
-  </si>
-  <si>
-    <t>2 horas</t>
-  </si>
-  <si>
-    <t>4.5 horas</t>
-  </si>
-  <si>
-    <t>8.2 horas</t>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Diseñó la interfaz de la página de inicio</t>
+  </si>
+  <si>
+    <t>Definió la estructura de la base de datos</t>
+  </si>
+  <si>
+    <t>Carrito</t>
+  </si>
+  <si>
+    <t>Estableció la funcionalidad del carrito de compras</t>
+  </si>
+  <si>
+    <t>Pagos</t>
+  </si>
+  <si>
+    <t>Propuso el flujo de pago y validaciones</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>1.5h</t>
+  </si>
+  <si>
+    <t>Inicio del documento del corte y Fase de Design Studio</t>
+  </si>
+  <si>
+    <t>3.35</t>
+  </si>
+  <si>
+    <t>Creación de Design Studio y todas sus fases</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelación de Prototipado y Disusciones </t>
+  </si>
+  <si>
+    <t>2.15h</t>
+  </si>
+  <si>
+    <t>Conferencias con clientes para las bitácoras y confirmaciones</t>
+  </si>
+  <si>
+    <t>Mapa de Historias de Usuario para Clientes</t>
+  </si>
+  <si>
+    <t>0.30h</t>
+  </si>
+  <si>
+    <t>Finalización de Documento y Creación de Presentación</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +503,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -394,22 +529,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -418,22 +542,33 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,32 +912,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{146D5FA7-A809-429D-BF8A-20F60175E49B}">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="74" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.9140625" customWidth="1"/>
-    <col min="2" max="2" width="10.89453125" customWidth="1"/>
-    <col min="3" max="3" width="9.14453125" customWidth="1"/>
-    <col min="4" max="4" width="23.40625" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
-    <col min="6" max="6" width="10.35546875" customWidth="1"/>
-    <col min="7" max="7" width="46.41015625" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="46.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -810,7 +945,7 @@
         <v>23968</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -833,9 +968,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
-        <v>45685</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11">
+        <v>45700</v>
       </c>
       <c r="B6" s="7">
         <v>0.48194444444444445</v>
@@ -856,9 +991,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>45686</v>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11">
+        <v>45701</v>
       </c>
       <c r="B7" s="7">
         <v>0.49444444444444446</v>
@@ -879,9 +1014,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>45686</v>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11">
+        <v>45702</v>
       </c>
       <c r="B8" s="7">
         <v>0.68333333333333335</v>
@@ -902,9 +1037,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>45686</v>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11">
+        <v>45703</v>
       </c>
       <c r="B9" s="7">
         <v>0.6875</v>
@@ -925,9 +1060,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>45690</v>
+    <row r="10" spans="1:7" ht="28.9">
+      <c r="A10" s="11">
+        <v>45704</v>
       </c>
       <c r="B10" s="7">
         <v>0.92569444444444449</v>
@@ -944,79 +1079,135 @@
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>45691</v>
-      </c>
-      <c r="B11" s="7">
+    <row r="11" spans="1:7">
+      <c r="A11" s="11">
+        <v>45705</v>
+      </c>
+      <c r="B11" s="15">
         <v>0.50694444444444442</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="15">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="16">
         <v>1</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15">
+      <c r="A12" s="11">
+        <v>45706</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15">
+      <c r="A13" s="11">
+        <v>45708</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.6875</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15">
+      <c r="A14" s="11">
+        <v>45711</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15">
+      <c r="A15" s="11">
+        <v>45713</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.4375</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1025,7 +1216,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1034,7 +1225,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1043,7 +1234,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1052,7 +1243,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1061,7 +1252,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1070,7 +1261,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1079,7 +1270,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1088,7 +1279,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1097,7 +1288,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1106,7 +1297,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1128,32 +1319,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1058A76E-730D-4D76-A061-46B23C3712B2}">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.9140625" customWidth="1"/>
-    <col min="2" max="2" width="10.89453125" customWidth="1"/>
-    <col min="3" max="3" width="9.14453125" customWidth="1"/>
-    <col min="4" max="4" width="23.40625" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
-    <col min="6" max="6" width="16.6796875" customWidth="1"/>
-    <col min="7" max="7" width="47.484375" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="47.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1161,32 +1352,32 @@
         <v>23202</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>28</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11">
+        <v>45701</v>
       </c>
       <c r="B6" s="7">
         <v>0.79166666666666663</v>
@@ -1195,67 +1386,67 @@
         <v>0.80208333333333337</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="16">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11">
+        <v>45702</v>
+      </c>
+      <c r="B7" s="6">
         <v>0.8125</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="6">
         <v>0.82638888888888884</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="17">
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11">
+        <v>45703</v>
+      </c>
+      <c r="B8" s="6">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="6">
         <v>0.99305555555555558</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
+      <c r="D8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11">
+        <v>45704</v>
       </c>
       <c r="B9" s="6">
         <v>0.41666666666666669</v>
@@ -1264,71 +1455,139 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="11">
+        <v>45705</v>
+      </c>
+      <c r="B10" s="20">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C10" s="20">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" ht="15">
+      <c r="A11" s="11">
+        <v>45706</v>
+      </c>
+      <c r="B11" s="12">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15">
+      <c r="A12" s="11">
+        <v>45707</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.6875</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15">
+      <c r="A13" s="11">
+        <v>45709</v>
+      </c>
+      <c r="B13" s="12">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15">
+      <c r="A14" s="11">
+        <v>45711</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1337,7 +1596,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1346,7 +1605,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1355,7 +1614,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1364,7 +1623,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1373,7 +1632,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1382,7 +1641,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1391,7 +1650,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1400,7 +1659,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1409,7 +1668,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1418,7 +1677,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1427,7 +1686,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1449,32 +1708,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45D095D-13A7-403C-968C-DCAAF7347694}">
   <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="74" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.9140625" customWidth="1"/>
-    <col min="2" max="2" width="10.89453125" customWidth="1"/>
-    <col min="3" max="3" width="9.14453125" customWidth="1"/>
-    <col min="4" max="4" width="23.40625" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
-    <col min="6" max="6" width="10.35546875" customWidth="1"/>
-    <col min="7" max="7" width="81.25" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="81.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1482,7 +1741,7 @@
         <v>23247</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1505,9 +1764,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11">
+        <v>45698</v>
       </c>
       <c r="B6" s="7">
         <v>0.81944444444444442</v>
@@ -1516,22 +1775,22 @@
         <v>0.8618055555555556</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="E6" s="7">
-        <f>(C6-B6)</f>
+        <f t="shared" ref="E6:E27" si="0">(C6-B6)</f>
         <v>4.2361111111111183E-2</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>45659</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11">
+        <v>45699</v>
       </c>
       <c r="B7" s="7">
         <v>0.54513888888888884</v>
@@ -1540,22 +1799,22 @@
         <v>0.59027777777777779</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E7" s="7">
-        <f>(C7-B7)</f>
+        <f t="shared" si="0"/>
         <v>4.5138888888888951E-2</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>45690</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11">
+        <v>45700</v>
       </c>
       <c r="B8" s="7">
         <v>0.97777777777777775</v>
@@ -1564,22 +1823,22 @@
         <v>0.99305555555555558</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E8" s="7">
-        <f>(C8-B8)</f>
+        <f t="shared" si="0"/>
         <v>1.5277777777777835E-2</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>45718</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11">
+        <v>45701</v>
       </c>
       <c r="B9" s="7">
         <v>0.38541666666666669</v>
@@ -1588,22 +1847,22 @@
         <v>0.43055555555555558</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="E9" s="7">
-        <f>(C9-B9)</f>
+        <f t="shared" si="0"/>
         <v>4.5138888888888895E-2</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>45718</v>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="11">
+        <v>45702</v>
       </c>
       <c r="B10" s="7">
         <v>0.46180555555555558</v>
@@ -1612,22 +1871,22 @@
         <v>0.49861111111111112</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E10" s="7">
-        <f>(C10-B10)</f>
+        <f t="shared" si="0"/>
         <v>3.6805555555555536E-2</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>45718</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="11">
+        <v>45703</v>
       </c>
       <c r="B11" s="7">
         <v>0.58611111111111114</v>
@@ -1636,22 +1895,22 @@
         <v>0.61805555555555558</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="E11" s="7">
-        <f>(C11-B11)</f>
+        <f t="shared" si="0"/>
         <v>3.1944444444444442E-2</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>45718</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="11">
+        <v>45704</v>
       </c>
       <c r="B12" s="7">
         <v>0.95972222222222225</v>
@@ -1660,22 +1919,22 @@
         <v>0.97430555555555554</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E12" s="7">
-        <f>(C12-B12)</f>
+        <f t="shared" si="0"/>
         <v>1.4583333333333282E-2</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>45749</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="11">
+        <v>45705</v>
       </c>
       <c r="B13" s="7">
         <v>0.41666666666666669</v>
@@ -1684,194 +1943,238 @@
         <v>0.5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="E13" s="7">
-        <f>(C13-B13)</f>
+        <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>45749</v>
-      </c>
-      <c r="B14" s="7">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="11">
+        <v>45706</v>
+      </c>
+      <c r="B14" s="15">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="15">
         <v>0.86458333333333337</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="7">
-        <f>(C14-B14)</f>
+      <c r="D14" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="15">
+        <f t="shared" si="0"/>
         <v>3.125E-2</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="16">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="7">
-        <f>(C15-B15)</f>
+      <c r="G14" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15">
+      <c r="A15" s="11">
+        <v>45707</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.375</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="12">
+        <v>0.11805555555555555</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A16" s="11">
+        <v>45709</v>
+      </c>
+      <c r="B16" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0.11805555555555555</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15">
+      <c r="A17" s="11">
+        <v>45712</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0.11805555555555555</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15">
+      <c r="A18" s="11">
+        <v>45714</v>
+      </c>
+      <c r="B18" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0.11805555555555555</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="7">
-        <f>(C16-B16)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="7">
-        <f>(C17-B17)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="7">
-        <f>(C18-B18)</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="7">
-        <f>(C19-B19)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="7">
-        <f>(C20-B20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="7">
-        <f>(C21-B21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="7">
-        <f>(C22-B22)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="7">
-        <f>(C23-B23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="7">
-        <f>(C24-B24)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="7">
-        <f>(C25-B25)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="7">
-        <f>(C26-B26)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="7">
-        <f>(C27-B27)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27" s="1"/>
@@ -1888,34 +2191,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8B52A6-7892-4687-9E62-DE47D8659B94}">
-  <dimension ref="A2:G28"/>
+  <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.9140625" customWidth="1"/>
-    <col min="2" max="2" width="10.89453125" customWidth="1"/>
-    <col min="3" max="3" width="9.14453125" customWidth="1"/>
-    <col min="4" max="4" width="23.40625" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
-    <col min="6" max="6" width="10.35546875" customWidth="1"/>
-    <col min="7" max="7" width="81.1171875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="81.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1923,21 +2226,21 @@
         <v>23201</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1960,9 +2263,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>51</v>
+    <row r="6" spans="1:7">
+      <c r="A6" s="11">
+        <v>45695</v>
       </c>
       <c r="B6" s="7">
         <v>0.25833333333333336</v>
@@ -1981,12 +2284,12 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="11">
+        <v>45696</v>
       </c>
       <c r="B7" s="7">
         <v>0.22847222222222222</v>
@@ -2005,12 +2308,12 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="11">
+        <v>45697</v>
       </c>
       <c r="B8" s="7">
         <v>0.36944444444444446</v>
@@ -2028,12 +2331,12 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="11">
+        <v>45698</v>
       </c>
       <c r="B9" s="7">
         <v>0.76458333333333328</v>
@@ -2045,19 +2348,19 @@
         <v>0.1</v>
       </c>
       <c r="E9" s="7">
-        <f>C9-B9</f>
+        <f t="shared" ref="E9:E16" si="0">C9-B9</f>
         <v>5.4861111111111138E-2</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="11">
+        <v>45699</v>
       </c>
       <c r="B10" s="7">
         <v>0.81597222222222221</v>
@@ -2069,19 +2372,19 @@
         <v>0</v>
       </c>
       <c r="E10" s="7">
-        <f>C10-B10</f>
+        <f t="shared" si="0"/>
         <v>4.5833333333333393E-2</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="11">
+        <v>45700</v>
       </c>
       <c r="B11" s="7">
         <v>0.37847222222222221</v>
@@ -2093,19 +2396,19 @@
         <v>0</v>
       </c>
       <c r="E11" s="7">
-        <f>C11-B11</f>
+        <f t="shared" si="0"/>
         <v>6.1111111111111116E-2</v>
       </c>
       <c r="F11" s="1">
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>45658</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="11">
+        <v>45701</v>
       </c>
       <c r="B12" s="7">
         <v>0.7416666666666667</v>
@@ -2117,19 +2420,19 @@
         <v>0.2</v>
       </c>
       <c r="E12" s="7">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>5.4166666666666585E-2</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>45689</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="11">
+        <v>45702</v>
       </c>
       <c r="B13" s="7">
         <v>0.55902777777777779</v>
@@ -2141,19 +2444,19 @@
         <v>0</v>
       </c>
       <c r="E13" s="7">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>3.819444444444442E-2</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>45689</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="11">
+        <v>45703</v>
       </c>
       <c r="B14" s="7">
         <v>0.92708333333333337</v>
@@ -2165,19 +2468,19 @@
         <v>0.05</v>
       </c>
       <c r="E14" s="7">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>4.513888888888884E-2</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
-        <v>45717</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="11">
+        <v>45704</v>
       </c>
       <c r="B15" s="7">
         <v>0.2638888888888889</v>
@@ -2189,131 +2492,271 @@
         <v>0.15</v>
       </c>
       <c r="E15" s="7">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>45748</v>
-      </c>
-      <c r="B16" s="7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="11">
+        <v>45705</v>
+      </c>
+      <c r="B16" s="15">
         <v>0.72222222222222221</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="15">
         <v>0.76736111111111116</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="16">
         <v>0.1</v>
       </c>
-      <c r="E16" s="7">
-        <f>C16-B16</f>
+      <c r="E16" s="15">
+        <f t="shared" si="0"/>
         <v>4.5138888888888951E-2</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <v>1</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G16" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15">
+      <c r="A17" s="11">
+        <v>45706</v>
+      </c>
+      <c r="B17" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="13">
+        <v>0</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15">
+      <c r="A18" s="11">
+        <v>45708</v>
+      </c>
+      <c r="B18" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D18" s="13">
+        <v>0</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15">
+      <c r="A19" s="11">
+        <v>45710</v>
+      </c>
+      <c r="B19" s="12">
+        <v>0.375</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D19" s="13">
+        <v>0</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15">
+      <c r="A20" s="11">
+        <v>45713</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D20" s="13">
+        <v>0</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="23">
+        <v>45704</v>
+      </c>
+      <c r="B21" s="18">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="17">
+        <v>2</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="24">
+        <v>45705</v>
+      </c>
+      <c r="B22" s="7">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="C22" s="7">
+        <v>0.28819444444444442</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="24">
+        <v>45707</v>
+      </c>
+      <c r="B23" s="7">
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.1423611111111111</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="24">
+        <v>45710</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.25694444444444442</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15">
+      <c r="A25" s="24">
+        <v>45713</v>
+      </c>
+      <c r="B25" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>6.25E-2</v>
+      </c>
+      <c r="F25" s="1">
+        <v>2</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15">
+      <c r="A26" s="24">
+        <v>45714</v>
+      </c>
+      <c r="B26" s="7">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C26" s="7">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2322,7 +2765,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2330,6 +2773,15 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" ht="15">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2341,23 +2793,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5f200c4c-69ef-4d05-97e7-d19860507b1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010070E446D4C204484A80D739847D4B1F5E" ma:contentTypeVersion="14" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4438d9b8ff6b847ab586b35b6edc2567">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5f200c4c-69ef-4d05-97e7-d19860507b1d" xmlns:ns4="f379af12-142c-4b6c-a2a9-ff9d91561f10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="29b332170284ab190cf2d7ab9f1e59db" ns3:_="" ns4:_="">
     <xsd:import namespace="5f200c4c-69ef-4d05-97e7-d19860507b1d"/>
@@ -2584,34 +3019,31 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5f200c4c-69ef-4d05-97e7-d19860507b1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39D0DA3D-26CE-49A3-AD71-7EBC78F4879C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="5f200c4c-69ef-4d05-97e7-d19860507b1d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EFF80D3-E423-4DE5-AD75-C696A25AA072}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6F67F74-E666-4985-B0E5-25ED104A07FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39D0DA3D-26CE-49A3-AD71-7EBC78F4879C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EFF80D3-E423-4DE5-AD75-C696A25AA072}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="5f200c4c-69ef-4d05-97e7-d19860507b1d"/>
-    <ds:schemaRef ds:uri="f379af12-142c-4b6c-a2a9-ff9d91561f10"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6F67F74-E666-4985-B0E5-25ED104A07FF}"/>
 </file>
</xml_diff>